<commit_message>
model running is now functionalized, results computes and SA table produced
</commit_message>
<xml_diff>
--- a/input-data.xlsx
+++ b/input-data.xlsx
@@ -519,7 +519,7 @@
   <dimension ref="A1:BB83"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K7" sqref="K7"/>
+      <selection activeCell="I12" sqref="I12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1392,7 +1392,7 @@
       <c r="F7" s="7">
         <v>0.125</v>
       </c>
-      <c r="G7" s="4">
+      <c r="G7" s="7">
         <f t="shared" si="0"/>
         <v>0.245</v>
       </c>
@@ -1551,7 +1551,7 @@
       <c r="F8" s="7">
         <v>0.125</v>
       </c>
-      <c r="G8" s="4">
+      <c r="G8" s="7">
         <f t="shared" si="0"/>
         <v>0.27500000000000002</v>
       </c>
@@ -1710,7 +1710,7 @@
       <c r="F9" s="7">
         <v>0.125</v>
       </c>
-      <c r="G9" s="4">
+      <c r="G9" s="7">
         <f t="shared" si="0"/>
         <v>0.30499999999999999</v>
       </c>
@@ -1869,7 +1869,7 @@
       <c r="F10" s="7">
         <v>0.125</v>
       </c>
-      <c r="G10" s="4">
+      <c r="G10" s="7">
         <f t="shared" si="0"/>
         <v>0.33499999999999996</v>
       </c>
@@ -2028,7 +2028,7 @@
       <c r="F11" s="7">
         <v>0.125</v>
       </c>
-      <c r="G11" s="4">
+      <c r="G11" s="7">
         <f t="shared" si="0"/>
         <v>0.36499999999999999</v>
       </c>
@@ -2187,7 +2187,7 @@
       <c r="F12" s="7">
         <v>0.125</v>
       </c>
-      <c r="G12" s="4">
+      <c r="G12" s="7">
         <f t="shared" si="0"/>
         <v>0.39500000000000002</v>
       </c>
@@ -2346,7 +2346,7 @@
       <c r="F13" s="7">
         <v>0.125</v>
       </c>
-      <c r="G13" s="4">
+      <c r="G13" s="7">
         <f t="shared" si="0"/>
         <v>0.45500000000000002</v>
       </c>
@@ -2505,7 +2505,7 @@
       <c r="F14" s="7">
         <v>0.125</v>
       </c>
-      <c r="G14" s="4">
+      <c r="G14" s="7">
         <f t="shared" si="0"/>
         <v>0.51500000000000001</v>
       </c>
@@ -2664,7 +2664,7 @@
       <c r="F15" s="7">
         <v>0.125</v>
       </c>
-      <c r="G15" s="4">
+      <c r="G15" s="7">
         <f t="shared" si="0"/>
         <v>0.57499999999999996</v>
       </c>
@@ -3910,7 +3910,7 @@
       <c r="F23" s="6">
         <v>0.24</v>
       </c>
-      <c r="G23" s="4">
+      <c r="G23" s="6">
         <f t="shared" si="0"/>
         <v>0.4</v>
       </c>
@@ -4069,7 +4069,7 @@
       <c r="F24" s="6">
         <v>0.24</v>
       </c>
-      <c r="G24" s="4">
+      <c r="G24" s="6">
         <f t="shared" si="0"/>
         <v>0.43</v>
       </c>
@@ -4228,7 +4228,7 @@
       <c r="F25" s="6">
         <v>0.24</v>
       </c>
-      <c r="G25" s="4">
+      <c r="G25" s="6">
         <f t="shared" si="0"/>
         <v>0.45999999999999996</v>
       </c>
@@ -4387,7 +4387,7 @@
       <c r="F26" s="6">
         <v>0.24</v>
       </c>
-      <c r="G26" s="4">
+      <c r="G26" s="6">
         <f t="shared" si="0"/>
         <v>0.49</v>
       </c>
@@ -4546,7 +4546,7 @@
       <c r="F27" s="6">
         <v>0.24</v>
       </c>
-      <c r="G27" s="4">
+      <c r="G27" s="6">
         <f t="shared" si="0"/>
         <v>0.52</v>
       </c>
@@ -4705,7 +4705,7 @@
       <c r="F28" s="6">
         <v>0.24</v>
       </c>
-      <c r="G28" s="4">
+      <c r="G28" s="6">
         <f t="shared" si="0"/>
         <v>0.58000000000000007</v>
       </c>
@@ -4864,7 +4864,7 @@
       <c r="F29" s="6">
         <v>0.24</v>
       </c>
-      <c r="G29" s="4">
+      <c r="G29" s="6">
         <f t="shared" si="0"/>
         <v>0.64</v>
       </c>
@@ -5023,7 +5023,7 @@
       <c r="F30" s="6">
         <v>0.24</v>
       </c>
-      <c r="G30" s="4">
+      <c r="G30" s="6">
         <f t="shared" si="0"/>
         <v>0.7</v>
       </c>
@@ -5182,7 +5182,7 @@
       <c r="F31" s="6">
         <v>0.24</v>
       </c>
-      <c r="G31" s="4">
+      <c r="G31" s="6">
         <f t="shared" si="0"/>
         <v>0.76</v>
       </c>
@@ -6580,7 +6580,7 @@
       <c r="F40" s="6">
         <v>0.42</v>
       </c>
-      <c r="G40" s="4">
+      <c r="G40" s="6">
         <f t="shared" si="0"/>
         <v>0.51</v>
       </c>
@@ -6739,7 +6739,7 @@
       <c r="F41" s="6">
         <v>0.42</v>
       </c>
-      <c r="G41" s="4">
+      <c r="G41" s="6">
         <f t="shared" si="0"/>
         <v>0.54</v>
       </c>
@@ -6898,7 +6898,7 @@
       <c r="F42" s="6">
         <v>0.42</v>
       </c>
-      <c r="G42" s="4">
+      <c r="G42" s="6">
         <f t="shared" si="0"/>
         <v>0.56999999999999995</v>
       </c>
@@ -7057,7 +7057,7 @@
       <c r="F43" s="6">
         <v>0.42</v>
       </c>
-      <c r="G43" s="4">
+      <c r="G43" s="6">
         <f t="shared" si="0"/>
         <v>0.6</v>
       </c>
@@ -7216,7 +7216,7 @@
       <c r="F44" s="6">
         <v>0.42</v>
       </c>
-      <c r="G44" s="4">
+      <c r="G44" s="6">
         <f t="shared" si="0"/>
         <v>0.63</v>
       </c>
@@ -7375,7 +7375,7 @@
       <c r="F45" s="6">
         <v>0.42</v>
       </c>
-      <c r="G45" s="4">
+      <c r="G45" s="6">
         <f t="shared" si="0"/>
         <v>0.65999999999999992</v>
       </c>
@@ -7534,7 +7534,7 @@
       <c r="F46" s="6">
         <v>0.42</v>
       </c>
-      <c r="G46" s="4">
+      <c r="G46" s="6">
         <f t="shared" si="0"/>
         <v>0.72</v>
       </c>
@@ -7690,7 +7690,7 @@
       <c r="F47" s="6">
         <v>0.42</v>
       </c>
-      <c r="G47" s="4">
+      <c r="G47" s="6">
         <f t="shared" si="0"/>
         <v>0.78</v>
       </c>
@@ -9115,7 +9115,7 @@
       <c r="F56" s="6">
         <v>0.15</v>
       </c>
-      <c r="G56" s="4">
+      <c r="G56" s="6">
         <f t="shared" si="0"/>
         <v>0.27</v>
       </c>
@@ -9274,7 +9274,7 @@
       <c r="F57" s="6">
         <v>0.15</v>
       </c>
-      <c r="G57" s="4">
+      <c r="G57" s="6">
         <f t="shared" si="0"/>
         <v>0.3</v>
       </c>
@@ -9433,7 +9433,7 @@
       <c r="F58" s="6">
         <v>0.15</v>
       </c>
-      <c r="G58" s="4">
+      <c r="G58" s="6">
         <f t="shared" si="0"/>
         <v>0.32999999999999996</v>
       </c>
@@ -9592,7 +9592,7 @@
       <c r="F59" s="6">
         <v>0.15</v>
       </c>
-      <c r="G59" s="4">
+      <c r="G59" s="6">
         <f t="shared" si="0"/>
         <v>0.36</v>
       </c>
@@ -9751,7 +9751,7 @@
       <c r="F60" s="6">
         <v>0.15</v>
       </c>
-      <c r="G60" s="4">
+      <c r="G60" s="6">
         <f t="shared" si="0"/>
         <v>0.39</v>
       </c>
@@ -9910,7 +9910,7 @@
       <c r="F61" s="6">
         <v>0.15</v>
       </c>
-      <c r="G61" s="4">
+      <c r="G61" s="6">
         <f t="shared" si="0"/>
         <v>0.42000000000000004</v>
       </c>
@@ -10069,7 +10069,7 @@
       <c r="F62" s="6">
         <v>0.15</v>
       </c>
-      <c r="G62" s="4">
+      <c r="G62" s="6">
         <f t="shared" si="0"/>
         <v>0.48</v>
       </c>
@@ -10228,7 +10228,7 @@
       <c r="F63" s="6">
         <v>0.15</v>
       </c>
-      <c r="G63" s="4">
+      <c r="G63" s="6">
         <f t="shared" si="0"/>
         <v>0.54</v>
       </c>
@@ -11977,7 +11977,7 @@
       <c r="F74" s="6">
         <v>0.18</v>
       </c>
-      <c r="G74" s="4">
+      <c r="G74" s="6">
         <f t="shared" si="1"/>
         <v>0.32999999999999996</v>
       </c>
@@ -12136,7 +12136,7 @@
       <c r="F75" s="6">
         <v>0.18</v>
       </c>
-      <c r="G75" s="4">
+      <c r="G75" s="6">
         <f t="shared" si="1"/>
         <v>0.36</v>
       </c>
@@ -12295,7 +12295,7 @@
       <c r="F76" s="6">
         <v>0.18</v>
       </c>
-      <c r="G76" s="4">
+      <c r="G76" s="6">
         <f t="shared" si="1"/>
         <v>0.39</v>
       </c>
@@ -12454,7 +12454,7 @@
       <c r="F77" s="6">
         <v>0.18</v>
       </c>
-      <c r="G77" s="4">
+      <c r="G77" s="6">
         <f t="shared" si="1"/>
         <v>0.42</v>
       </c>
@@ -12613,7 +12613,7 @@
       <c r="F78" s="6">
         <v>0.18</v>
       </c>
-      <c r="G78" s="4">
+      <c r="G78" s="6">
         <f t="shared" si="1"/>
         <v>0.45</v>
       </c>
@@ -12772,7 +12772,7 @@
       <c r="F79" s="6">
         <v>0.18</v>
       </c>
-      <c r="G79" s="4">
+      <c r="G79" s="6">
         <f t="shared" si="1"/>
         <v>0.48</v>
       </c>
@@ -12931,7 +12931,7 @@
       <c r="F80" s="6">
         <v>0.18</v>
       </c>
-      <c r="G80" s="4">
+      <c r="G80" s="6">
         <f t="shared" si="1"/>
         <v>0.54</v>
       </c>
@@ -13090,7 +13090,7 @@
       <c r="F81" s="6">
         <v>0.18</v>
       </c>
-      <c r="G81" s="4">
+      <c r="G81" s="6">
         <f t="shared" si="1"/>
         <v>0.6</v>
       </c>
@@ -13249,7 +13249,7 @@
       <c r="F82" s="6">
         <v>0.18</v>
       </c>
-      <c r="G82" s="4">
+      <c r="G82" s="6">
         <f t="shared" si="1"/>
         <v>0.65999999999999992</v>
       </c>
@@ -13408,7 +13408,7 @@
       <c r="F83" s="6">
         <v>0.18</v>
       </c>
-      <c r="G83" s="4">
+      <c r="G83" s="6">
         <f t="shared" si="1"/>
         <v>0.72</v>
       </c>

</xml_diff>